<commit_message>
added new build files
</commit_message>
<xml_diff>
--- a/Source Materials/Vulcanus Max 40 3d printer BOM.xlsx
+++ b/Source Materials/Vulcanus Max 40 3d printer BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mobri\OneDrive\Documents\ElvanTechGit\vulcanusmax\Source Materials\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3C293AB4-1E03-4D45-B9B5-1EE2AD29D8AA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA1165A5-F309-4BF3-BFBA-FBE0641628A9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1650" yWindow="4245" windowWidth="25410" windowHeight="10755" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3315" yWindow="2910" windowWidth="27105" windowHeight="16650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="96">
   <si>
     <t>Qty</t>
   </si>
@@ -294,6 +294,21 @@
   <si>
     <t>Purchased</t>
   </si>
+  <si>
+    <t>banggood</t>
+  </si>
+  <si>
+    <t>ordered 3/30</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>received</t>
+  </si>
+  <si>
+    <t>reorder</t>
+  </si>
 </sst>
 </file>
 
@@ -302,7 +317,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -327,6 +342,12 @@
       <u/>
       <sz val="10"/>
       <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
       <name val="Arial"/>
     </font>
   </fonts>
@@ -365,10 +386,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -403,8 +425,12 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -722,7 +748,9 @@
   </sheetPr>
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -803,8 +831,12 @@
       <c r="B3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
+      <c r="F3" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>93</v>
+      </c>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
@@ -841,7 +873,9 @@
       <c r="E4" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="2"/>
+      <c r="F4" s="2" t="s">
+        <v>91</v>
+      </c>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
@@ -873,7 +907,9 @@
       <c r="C5" s="2"/>
       <c r="D5" s="1"/>
       <c r="E5" s="5"/>
-      <c r="F5" s="2"/>
+      <c r="F5" s="2" t="s">
+        <v>91</v>
+      </c>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
@@ -905,7 +941,9 @@
       <c r="C6" s="2"/>
       <c r="D6" s="1"/>
       <c r="E6" s="5"/>
-      <c r="F6" s="2"/>
+      <c r="F6" s="2" t="s">
+        <v>91</v>
+      </c>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
@@ -937,7 +975,9 @@
       <c r="C7" s="2"/>
       <c r="D7" s="1"/>
       <c r="E7" s="5"/>
-      <c r="F7" s="2"/>
+      <c r="F7" s="2" t="s">
+        <v>91</v>
+      </c>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
@@ -1007,8 +1047,12 @@
       <c r="E9" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
+      <c r="F9" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>95</v>
+      </c>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
@@ -1045,8 +1089,12 @@
       <c r="E10" s="5">
         <v>34.99</v>
       </c>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
+      <c r="F10" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>95</v>
+      </c>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
@@ -1077,8 +1125,12 @@
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
+      <c r="F11" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>95</v>
+      </c>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
@@ -1115,8 +1167,12 @@
       <c r="E12" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
+      <c r="F12" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>94</v>
+      </c>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
@@ -1153,7 +1209,9 @@
       <c r="E13" s="5">
         <v>4.1900000000000004</v>
       </c>
-      <c r="F13" s="2"/>
+      <c r="F13" s="2" t="s">
+        <v>91</v>
+      </c>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
@@ -1191,7 +1249,9 @@
       <c r="E14" s="5">
         <v>4.3899999999999997</v>
       </c>
-      <c r="F14" s="2"/>
+      <c r="F14" s="2" t="s">
+        <v>91</v>
+      </c>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
@@ -1229,7 +1289,9 @@
       <c r="E15" s="5">
         <v>3.99</v>
       </c>
-      <c r="F15" s="2"/>
+      <c r="F15" s="2" t="s">
+        <v>91</v>
+      </c>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
@@ -1267,8 +1329,12 @@
       <c r="E16" s="5">
         <v>15.99</v>
       </c>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
+      <c r="F16" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>95</v>
+      </c>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
@@ -1296,7 +1362,7 @@
       <c r="B17" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C17" s="12" t="s">
         <v>35</v>
       </c>
       <c r="D17" s="1">
@@ -1417,8 +1483,12 @@
       <c r="E20" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
+      <c r="F20" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>95</v>
+      </c>
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
@@ -1455,8 +1525,12 @@
       <c r="E21" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
+      <c r="F21" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>95</v>
+      </c>
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
@@ -1531,7 +1605,9 @@
       <c r="E23" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="F23" s="2"/>
+      <c r="F23" s="2" t="s">
+        <v>91</v>
+      </c>
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
       <c r="I23" s="2"/>
@@ -1645,8 +1721,12 @@
       <c r="E26" s="5">
         <v>3.96</v>
       </c>
-      <c r="F26" s="2"/>
-      <c r="G26" s="2"/>
+      <c r="F26" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>94</v>
+      </c>
       <c r="H26" s="2"/>
       <c r="I26" s="2"/>
       <c r="J26" s="2"/>
@@ -1942,7 +2022,9 @@
       <c r="E35" s="5">
         <v>6.09</v>
       </c>
-      <c r="F35" s="2"/>
+      <c r="F35" s="2" t="s">
+        <v>91</v>
+      </c>
       <c r="G35" s="2"/>
       <c r="H35" s="2"/>
       <c r="I35" s="2"/>
@@ -1980,7 +2062,9 @@
       <c r="E36" s="5">
         <v>8.99</v>
       </c>
-      <c r="F36" s="2"/>
+      <c r="F36" s="2" t="s">
+        <v>91</v>
+      </c>
       <c r="G36" s="2"/>
       <c r="H36" s="2"/>
       <c r="I36" s="2"/>
@@ -2018,7 +2102,9 @@
       <c r="E37" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="F37" s="2"/>
+      <c r="F37" s="2" t="s">
+        <v>91</v>
+      </c>
       <c r="G37" s="2"/>
       <c r="H37" s="2"/>
       <c r="I37" s="2"/>

</xml_diff>